<commit_message>
add confirmation if condition in request
</commit_message>
<xml_diff>
--- a/Purpose List.xlsx
+++ b/Purpose List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="509">
   <si>
     <t>PURPOSE LIST</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>1.5MVA Transformer Overcurrent and Earthfault Protection Relay</t>
+    <t>1.5 MVA Transformer Overcurrent and Earthfault Protection Relay</t>
   </si>
   <si>
     <t>23 Additional CCTV Requirements at CENPRI Site</t>
@@ -62,6 +62,9 @@
     <t>Additional Layer for Cooling Tower Extension Concrete Manhole</t>
   </si>
   <si>
+    <t>Additional Materials for Connection of Pump &amp; PVC Riser Pipe and Discharge Line of Deep Well</t>
+  </si>
+  <si>
     <t>Additional Padlock for Reconditioning Equipment Tool Cabinet</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
     <t>Anti-Condensate Heater</t>
   </si>
   <si>
+    <t>Assembling &amp; Installation</t>
+  </si>
+  <si>
     <t>Assembling of lube oil cooler plate</t>
   </si>
   <si>
@@ -104,12 +110,18 @@
     <t>Automation of Centrifugal Pump in Fire Fighting Control System</t>
   </si>
   <si>
+    <t>Auxiliary Process Temperature Monitoring</t>
+  </si>
+  <si>
     <t>Backfilling / Ground Preparation / Canal Rip-rapping (1 side only)</t>
   </si>
   <si>
     <t>Battery Replacement for Digital Caliper and Depth Gauge</t>
   </si>
   <si>
+    <t>Battery Replacement for Electronic Deflection Gauge</t>
+  </si>
+  <si>
     <t>Bearing Replacement for Soft Water Pump Repair</t>
   </si>
   <si>
@@ -146,6 +158,9 @@
     <t>Cenpri Site Uniform for Admin Personnel</t>
   </si>
   <si>
+    <t>CENPRI Warehouse Beginning Balance</t>
+  </si>
+  <si>
     <t>Change Lubricating Oil</t>
   </si>
   <si>
@@ -158,9 +173,18 @@
     <t>Christmas Prizes</t>
   </si>
   <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Cleaning &amp; Preservation of Tools</t>
+  </si>
+  <si>
     <t>Cleaning and Hauling of bunker oil in A Bank and B Bank DG4 using Saw dust</t>
   </si>
   <si>
+    <t>Cleaning and Repainting of Raw Water Storage Tank Roof</t>
+  </si>
+  <si>
     <t>Cleaning and Repiping of Sludge Tank No. 2</t>
   </si>
   <si>
@@ -176,12 +200,21 @@
     <t>Configuration of EasyGen for Interlocking of Unit 4 &amp; 5 NGR</t>
   </si>
   <si>
+    <t>Configuration of SEPAM Relay</t>
+  </si>
+  <si>
     <t>Construction</t>
   </si>
   <si>
     <t>Construction of Canal in Right Bank of Engine Foundation</t>
   </si>
   <si>
+    <t>Construction of Canteen Railings and Mechanical Separator Cover</t>
+  </si>
+  <si>
+    <t>Construction of Cantilever Rip-Rap Wall at Main Drain Canal</t>
+  </si>
+  <si>
     <t>Construction of Cantilever Rip-Rap Wall at Main Drain Canal for Protection of Transmission Line Concrete Take Off Pole Foundation</t>
   </si>
   <si>
@@ -194,9 +227,15 @@
     <t>Consumable for Air Filter Motor Stator Rewinding</t>
   </si>
   <si>
+    <t>Consumable for Engine Driven Pump</t>
+  </si>
+  <si>
     <t>Consumable For Inspection of Crankpin Journal Bearing</t>
   </si>
   <si>
+    <t>Consumables for  Rewinding of Rotor Pole #2</t>
+  </si>
+  <si>
     <t>Consumables for Cleaning of Foundation Canal</t>
   </si>
   <si>
@@ -206,10 +245,13 @@
     <t>Consumables for Jacket Water Cooler Plates Servicing</t>
   </si>
   <si>
+    <t>Consumables for Lube Oil Cooler Plates Servicing</t>
+  </si>
+  <si>
     <t>Consumables for Servicing of Switchgear Enclosure</t>
   </si>
   <si>
-    <t>Consumables, Tools and Equipment's for Spare Stator Rewinding</t>
+    <t>Consumables, Tools and Equipment for Spare Stator Rewinding</t>
   </si>
   <si>
     <t>Consumption of Heavy Equipment (Bulk Transfer &amp; Re-positioning)</t>
@@ -234,6 +276,9 @@
     <t>Cover For MOCB Units</t>
   </si>
   <si>
+    <t>Crack Testing of Parts</t>
+  </si>
+  <si>
     <t>Crack Testing of Spare Jacket/Cylinder Liner</t>
   </si>
   <si>
@@ -246,12 +291,12 @@
     <t>Cylinder Head Hydraulic Tensioning Tool.</t>
   </si>
   <si>
-    <t>Cylinder Head, Lapping</t>
-  </si>
-  <si>
     <t>Deep cleaning, painting and preservation of tools and equipments (Additional)</t>
   </si>
   <si>
+    <t>Deep Well Water Filter</t>
+  </si>
+  <si>
     <t>DG # 1 Stator Winding Temparature Protection/ Monitoring</t>
   </si>
   <si>
@@ -270,6 +315,9 @@
     <t>Drilling of Damaged Bolt Holes.</t>
   </si>
   <si>
+    <t>ECMG Office Renovation</t>
+  </si>
+  <si>
     <t>EIC Consumables</t>
   </si>
   <si>
@@ -282,12 +330,18 @@
     <t>Enclosure and Termination of SEL 487B Bus Protection Relay</t>
   </si>
   <si>
+    <t>Endorse to Tool Keeper</t>
+  </si>
+  <si>
     <t>Engine Replacement and Spare Parts</t>
   </si>
   <si>
     <t>Environment/Pollution Control Consumables</t>
   </si>
   <si>
+    <t>Equipment Alignment</t>
+  </si>
+  <si>
     <t>Equipment NGCP Requirements</t>
   </si>
   <si>
@@ -303,15 +357,24 @@
     <t>Excess Materials</t>
   </si>
   <si>
+    <t>Exhaust Flange Repair, Pielstick</t>
+  </si>
+  <si>
     <t>Fabrication</t>
   </si>
   <si>
-    <t>Fabrication and Installation of DG1,2 &amp; 3 Generator Base Cover</t>
+    <t>Fabrication and Installation of Generator Base Cover</t>
   </si>
   <si>
     <t>Fabrication of 3 Sample Racks for Warehouse</t>
   </si>
   <si>
+    <t>Fabrication of 3 Steel Drum Cabinets &amp; 4 Drum Racks (3-Layered)</t>
+  </si>
+  <si>
+    <t>Fabrication of 6 pcs Garbage Bins To Be Donated to Brookside Garden Academy</t>
+  </si>
+  <si>
     <t>Fabrication of Air Cooler Hydrotesting Cover Plate</t>
   </si>
   <si>
@@ -321,7 +384,16 @@
     <t>Fabrication of Battery Rack for 125Vdc Battery (100Ah)</t>
   </si>
   <si>
-    <t>Fabrication of Expansion Belows</t>
+    <t>Fabrication of Column Anchor Bolts</t>
+  </si>
+  <si>
+    <t>Fabrication of Cooling Tower Fan Motor Cover</t>
+  </si>
+  <si>
+    <t>Fabrication of Equipment for Rotor Pole Rewinding</t>
+  </si>
+  <si>
+    <t>Fabrication of Expansion Bellows</t>
   </si>
   <si>
     <t>Fabrication of Fuel Rack Stopper</t>
@@ -333,6 +405,12 @@
     <t>Fabrication of Guying Equalizer Bodies</t>
   </si>
   <si>
+    <t>Fabrication of Hand Wheel</t>
+  </si>
+  <si>
+    <t>Fabrication of Jacket Water Cooler Ring Gasket</t>
+  </si>
+  <si>
     <t>Fabrication of Lifting Frame for 4 Units Generator</t>
   </si>
   <si>
@@ -342,7 +420,10 @@
     <t>Fabrication of Office Partition</t>
   </si>
   <si>
-    <t>Fabrication of Oil Ring Stopper for DG Units 1, 2 and 3 Pedestal Bearing</t>
+    <t>Fabrication of Oil Ring Stopper for Pedestal Bearing</t>
+  </si>
+  <si>
+    <t>Fabrication of Phenolic Flat Washer For Pedestal Bearing</t>
   </si>
   <si>
     <t>Fabrication of Platform and Ladder</t>
@@ -352,6 +433,12 @@
   </si>
   <si>
     <t>Fabrication of Starting/Relief Valve Blind Plugs</t>
+  </si>
+  <si>
+    <t>Fabrication of Storage Cabinet</t>
+  </si>
+  <si>
+    <t>Fabrication of Water Meter Manhole Cover</t>
   </si>
   <si>
     <t>Fabrication of Wooden Crates For Cylinder Head Assy &amp; Cylinder Liner To Be Shipped to Mindoro</t>
@@ -382,18 +469,39 @@
     <t>For Adjustment/Correction of Item Name</t>
   </si>
   <si>
+    <t>For After Transition Piece</t>
+  </si>
+  <si>
     <t>For Air Cooler Thread Repair</t>
   </si>
   <si>
+    <t>For Air Cooler Vent Valve</t>
+  </si>
+  <si>
     <t>For Blood Sugar Monitoring(Set 2) &amp; Clinic Supplies</t>
   </si>
   <si>
+    <t>For Common Use</t>
+  </si>
+  <si>
     <t>For Connecting 2 Reference Grounding Point (Microwave Tower - Substation) to Prevent Potential Difference for the Microwave Device Protection</t>
   </si>
   <si>
+    <t>For Control Circuit Labelling in MCCS, Switchgear Enclosure</t>
+  </si>
+  <si>
+    <t>For Cooling Tower Fan Motor</t>
+  </si>
+  <si>
+    <t>For Cooling Tower Fan Motor, Gear Box &amp; Housing</t>
+  </si>
+  <si>
     <t>For Earthing Conductor at Tank Farm Area to Discharge Electrostatic during Lightning</t>
   </si>
   <si>
+    <t>For Engine Driven Relief Valve</t>
+  </si>
+  <si>
     <t>For Environment Department Use.</t>
   </si>
   <si>
@@ -403,9 +511,18 @@
     <t>For Jacking Bolt</t>
   </si>
   <si>
+    <t>For Lighting Surge Protection System</t>
+  </si>
+  <si>
     <t>For Office Documentation Use</t>
   </si>
   <si>
+    <t>For Operation of Engine Driven Pump</t>
+  </si>
+  <si>
+    <t>For Portable Back-up Storage of Important Projects &amp; Office Files / Documents</t>
+  </si>
+  <si>
     <t>For Shells(Waste Heat Recovery Boilers Removal)</t>
   </si>
   <si>
@@ -415,27 +532,54 @@
     <t>For Spare Unit on 125 VDC Battery, Bank for Generator</t>
   </si>
   <si>
+    <t>For Temperature Monitoring Instrument</t>
+  </si>
+  <si>
     <t>For The Use on 8PC2-5 (Talisay Engine Inspection)</t>
   </si>
   <si>
-    <t>For Turbo Drain Charger</t>
+    <t>For Turbo Charger Air Intake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For Turbo Charger Drain </t>
   </si>
   <si>
     <t>For Use In Common Bus Differential Fault &amp; Breaker Failure Protection</t>
   </si>
   <si>
+    <t>For Use in FOM#3 Feed Pump Motor Controller</t>
+  </si>
+  <si>
     <t>For Use in Generator Control Panel (Auto Loading &amp; Auto Synchronization Function)</t>
   </si>
   <si>
     <t>For use in Lightning Strikes Monitoring, Interface on Microwave Antenna Lightning Protection System</t>
   </si>
   <si>
+    <t>For Use In Sludge Pump Motor Stator Rewinding</t>
+  </si>
+  <si>
+    <t>For XLPE Cable #2 Overwrap Protection on Termination</t>
+  </si>
+  <si>
     <t>Foundation &amp; Enclosure</t>
   </si>
   <si>
+    <t>Fuel Consumption</t>
+  </si>
+  <si>
+    <t>Fuel Drip &amp; Circulation</t>
+  </si>
+  <si>
     <t>Fuel For Rental of 0.3 cubic meter Bucket Backhoe</t>
   </si>
   <si>
+    <t>Fuel Injector Cooling Modification</t>
+  </si>
+  <si>
+    <t>Generator Base Thread Repair</t>
+  </si>
+  <si>
     <t>Generator Sliding Tools for Sulzer</t>
   </si>
   <si>
@@ -448,6 +592,9 @@
     <t>Governor Maintenance Tools</t>
   </si>
   <si>
+    <t>Governor Shut Down Device</t>
+  </si>
+  <si>
     <t>Grounding Installation for Microwave Antenna</t>
   </si>
   <si>
@@ -457,6 +604,12 @@
     <t>Grounding System Lay-out / Installation</t>
   </si>
   <si>
+    <t>Heater Protection</t>
+  </si>
+  <si>
+    <t>Heating of Auxiliary Generator</t>
+  </si>
+  <si>
     <t>HFO Fuel Piping Insulation</t>
   </si>
   <si>
@@ -478,9 +631,15 @@
     <t>Identification, Pre-Cleaning &amp; Tagging of Spare Parts for PIELSTICK Engine, at CV Area (Additional )</t>
   </si>
   <si>
+    <t>Injector Cooling Connector</t>
+  </si>
+  <si>
     <t>Injector Thread Repair</t>
   </si>
   <si>
+    <t>Injector Thread Repair Tools</t>
+  </si>
+  <si>
     <t>Inspection of Generator Stator Frame</t>
   </si>
   <si>
@@ -490,9 +649,15 @@
     <t>Installation and Fabrication</t>
   </si>
   <si>
+    <t>Installation and lay-out of Feeder Sludge Tank Heater</t>
+  </si>
+  <si>
     <t>Installation in Engine Drain Line</t>
   </si>
   <si>
+    <t>Installation of 13 Pcs Pressure Gauge in Fire Hydrant Cabinet, Sprinkler System</t>
+  </si>
+  <si>
     <t>Installation of 5 Units Flood Lights Inside Power Plant Area</t>
   </si>
   <si>
@@ -502,15 +667,27 @@
     <t>Installation of AC Powered Navigational Warning Light Flashing(as per insurance requirement)</t>
   </si>
   <si>
+    <t>Installation of Additional Anti-Condensate Heater</t>
+  </si>
+  <si>
     <t>Installation of Air Terminal</t>
   </si>
   <si>
+    <t>Installation of Air Vent for Charged Air Cooler</t>
+  </si>
+  <si>
     <t>Installation of Auxiliary Area Electrical Cable Plug</t>
   </si>
   <si>
     <t>Installation of Auxiliary Lighting Panel</t>
   </si>
   <si>
+    <t>Installation of Blind Flange</t>
+  </si>
+  <si>
+    <t>Installation of Bowl Motor Protection</t>
+  </si>
+  <si>
     <t>Installation of Breaker</t>
   </si>
   <si>
@@ -520,6 +697,9 @@
     <t>Installation of Canopy at 750kVA Transformer Protection Shed</t>
   </si>
   <si>
+    <t>Installation of Canopy at Exit Door Powerhouse Building Switch Gear Area</t>
+  </si>
+  <si>
     <t>Installation of Centrifugal Pump at Tank Farm Sump Pit</t>
   </si>
   <si>
@@ -532,12 +712,33 @@
     <t>Installation of Current Transformer Support for Bus Differential Fault Protection</t>
   </si>
   <si>
+    <t>Installation of Deep Well Pump-Motor Feeder Raceway</t>
+  </si>
+  <si>
+    <t>Installation of Discharge Line Form Mono Pump To Sludge Tank</t>
+  </si>
+  <si>
+    <t>Installation of Easygen Relay</t>
+  </si>
+  <si>
+    <t>Installation Of Electrical Main Distribution Panel For Auxiliary Load</t>
+  </si>
+  <si>
     <t>Installation of Expansion Bellow at Exhaust Main Header Pipe</t>
   </si>
   <si>
+    <t>Installation of Grounding Panel</t>
+  </si>
+  <si>
+    <t>Installation of Isolation Valve</t>
+  </si>
+  <si>
     <t>Installation of Jacket Water Cooler Plates Gasket</t>
   </si>
   <si>
+    <t>Installation of Lighting Arrester</t>
+  </si>
+  <si>
     <t>Installation of Microwave Control Panel at SCADA Room</t>
   </si>
   <si>
@@ -550,18 +751,30 @@
     <t>Installation of Overflow at Sludge Tanks</t>
   </si>
   <si>
+    <t>Installation of Padlock for Security</t>
+  </si>
+  <si>
     <t>Installation of Piping in Cooling Tower Drain Chamber-Extension</t>
   </si>
   <si>
     <t>Installation of Pippings</t>
   </si>
   <si>
+    <t>Installation of Power Supply of Auxiliary Generator Battery Charging</t>
+  </si>
+  <si>
     <t>Installation of Powerhouse Rear Wall Sun Panels</t>
   </si>
   <si>
     <t>Installation of Protection Relay</t>
   </si>
   <si>
+    <t>Installation of Remote Control</t>
+  </si>
+  <si>
+    <t>Installation of Remote Switch for LFO Day Tank</t>
+  </si>
+  <si>
     <t>Installation of SEL 487B Relay</t>
   </si>
   <si>
@@ -583,6 +796,9 @@
     <t>Installation of Test Block</t>
   </si>
   <si>
+    <t>Installation of Y-Strainers and Check Valves</t>
+  </si>
+  <si>
     <t>Installation, Testing &amp; Commissioning of the Automatic Fire Suppression System for the Engine Room</t>
   </si>
   <si>
@@ -607,18 +823,27 @@
     <t>Inventory, Preservation, and Tagging</t>
   </si>
   <si>
+    <t>Jacket Water Recovery System</t>
+  </si>
+  <si>
     <t>Labelling Content in Engine Fuel Tank</t>
   </si>
   <si>
     <t>Laboratory Use</t>
   </si>
   <si>
+    <t>Lapping of Cylinder Head</t>
+  </si>
+  <si>
     <t>Leadership Training</t>
   </si>
   <si>
     <t>Lifting Heavy Parts/Items in the Warehouse.</t>
   </si>
   <si>
+    <t>Lighting of Cable Trench</t>
+  </si>
+  <si>
     <t>Lightings</t>
   </si>
   <si>
@@ -637,18 +862,27 @@
     <t>Machining &amp; Fabrication of Unit 1 Lube Oil Priming Pump Shaft(Replacement to Damage Shaft)</t>
   </si>
   <si>
+    <t>Main Engine Frame Cleaning and Preserving</t>
+  </si>
+  <si>
     <t>Maintenance &amp; Reconditioning</t>
   </si>
   <si>
     <t>Maintenance Consumable for Assembling and Alignment</t>
   </si>
   <si>
-    <t>Maintenance Tools</t>
+    <t>Maintenance of Common Tools</t>
   </si>
   <si>
     <t>Material Recovery</t>
   </si>
   <si>
+    <t>Materials for Spare Stator Rewinding</t>
+  </si>
+  <si>
+    <t>Materials For Water Valve Block</t>
+  </si>
+  <si>
     <t>Measuring of Slot Width for Spare Stator Rewinding.</t>
   </si>
   <si>
@@ -667,9 +901,18 @@
     <t>Modification of Electrical Panel for Testing Equipment Storage.</t>
   </si>
   <si>
+    <t>Modification of Injector Cooling Nozzle Pipe Line</t>
+  </si>
+  <si>
+    <t>Modification of Main Bearing Sensor Cable Raceway</t>
+  </si>
+  <si>
     <t>Modification of Oil and Water Mechanical Separator Basin</t>
   </si>
   <si>
+    <t>Modification of Site Pesonnel Staff House Comfort Room</t>
+  </si>
+  <si>
     <t>New Station Service Transformer</t>
   </si>
   <si>
@@ -691,18 +934,30 @@
     <t>Online Monitoring &amp; Alarm</t>
   </si>
   <si>
+    <t>Operation Communication, Hand Held Radio/2way Radio</t>
+  </si>
+  <si>
     <t>Operations &amp; Maintenance Consumables</t>
   </si>
   <si>
+    <t>Oven Structure for Main Field &amp; Exciter Servicing</t>
+  </si>
+  <si>
     <t>Paint Removal</t>
   </si>
   <si>
     <t>Painting of Transition Piece</t>
   </si>
   <si>
+    <t>Painting of Turbo Charger Casing</t>
+  </si>
+  <si>
     <t>Painting Works</t>
   </si>
   <si>
+    <t>Parts for Replacement for DG1 &amp; DG3 Westfalia OSC15 Lube Oil Purifiers</t>
+  </si>
+  <si>
     <t>Personal Protective Equipment</t>
   </si>
   <si>
@@ -718,6 +973,9 @@
     <t>Plant Decorations</t>
   </si>
   <si>
+    <t>Planting Material For Demo Farm at Plant Site</t>
+  </si>
+  <si>
     <t>PMS (1000 R-Hrs)</t>
   </si>
   <si>
@@ -748,6 +1006,12 @@
     <t>Post Insulator Support</t>
   </si>
   <si>
+    <t>Power Back-up for Desktop Computers</t>
+  </si>
+  <si>
+    <t>Power Backup &amp; Power Surge</t>
+  </si>
+  <si>
     <t>Power House Enclosure - Phase 1</t>
   </si>
   <si>
@@ -757,6 +1021,9 @@
     <t>Power Supply</t>
   </si>
   <si>
+    <t>Powerhouse Comfort Room</t>
+  </si>
+  <si>
     <t>Powerhouse Ventilation: Phase 1 - Installation of Louvers</t>
   </si>
   <si>
@@ -769,9 +1036,15 @@
     <t>Preservation of Boiler Waste Heat Recovery</t>
   </si>
   <si>
+    <t>Preventive Maintenance For Lube Oil Separator</t>
+  </si>
+  <si>
     <t>Progen Consumables</t>
   </si>
   <si>
+    <t>Protection / Monitoring of Main Stator Winding Temperature</t>
+  </si>
+  <si>
     <t>Pump For Bleach / Chlorine To Be Used In 3DTrasar</t>
   </si>
   <si>
@@ -787,6 +1060,12 @@
     <t>Re-Painting of Engine Platform</t>
   </si>
   <si>
+    <t>Re-routing of Electric Wires</t>
+  </si>
+  <si>
+    <t>Re-Threading of Cylinder Head</t>
+  </si>
+  <si>
     <t>Ready Spare for 3 Units Sulzer Engines (Speed Sensor Generator)</t>
   </si>
   <si>
@@ -796,21 +1075,42 @@
     <t>Reconditioning</t>
   </si>
   <si>
+    <t>Reconditioning Area Fence</t>
+  </si>
+  <si>
+    <t>Reconditioning of Cylinder Liners</t>
+  </si>
+  <si>
     <t>Reconditioning of Lube Oil Cooler, Unit 5</t>
   </si>
   <si>
     <t>Rectification of Charger Air Cooler Chamber Gas Leak</t>
   </si>
   <si>
+    <t>Refill</t>
+  </si>
+  <si>
     <t>Refill Hydraulic Oil</t>
   </si>
   <si>
+    <t>Refuel</t>
+  </si>
+  <si>
     <t>Refuel for Heavy Equipment</t>
   </si>
   <si>
     <t>Removal &amp; Transfer of Mechanical Barracks</t>
   </si>
   <si>
+    <t>Removal of Bladder Pumps, Water Intake Pumps, Accessories and Structures</t>
+  </si>
+  <si>
+    <t>Removal of Boiler SEM Water Softener Module, Accessories and Structures</t>
+  </si>
+  <si>
+    <t>Removal of NCH Temporary Shed and Repair of Water Softener Storage Tank, Piping &amp; Pressure Tank Base Platform</t>
+  </si>
+  <si>
     <t>Renovation</t>
   </si>
   <si>
@@ -823,12 +1123,27 @@
     <t>Repainting of Air Cooler Casing and Turbocharger</t>
   </si>
   <si>
+    <t>Repainting of Air Intake Manifold Pipe</t>
+  </si>
+  <si>
+    <t>Repainting of Exhaust Main Header</t>
+  </si>
+  <si>
     <t>Repainting Works</t>
   </si>
   <si>
+    <t>Repair &amp; Servicing Works</t>
+  </si>
+  <si>
     <t>Repair and Maintenance</t>
   </si>
   <si>
+    <t>Repair and Modification of Defective Roofing, Gutters, Downspout Ridge Roll and Flashing</t>
+  </si>
+  <si>
+    <t>Repair and Repainting Exhaust Main Header and Retouching of Smokestack.</t>
+  </si>
+  <si>
     <t>Repair of Air Leak and Re-Gasketing of Air Duct Consumables</t>
   </si>
   <si>
@@ -841,6 +1156,12 @@
     <t>Repair of Fabricated Racks for Sulzer &amp; Pielstick Spareparts</t>
   </si>
   <si>
+    <t>Repair of Fuel Module Pump #2</t>
+  </si>
+  <si>
+    <t>Repair of Leaking BACIWAD Pipeline</t>
+  </si>
+  <si>
     <t>Repair of Leaking Powerhouse Roofing</t>
   </si>
   <si>
@@ -850,30 +1171,69 @@
     <t>Repair of Left Bank Condition Canal</t>
   </si>
   <si>
+    <t>Repair of Mechanical Staff House at Plant Site</t>
+  </si>
+  <si>
+    <t>Repair of Stairway Railings</t>
+  </si>
+  <si>
     <t>Replacement</t>
   </si>
   <si>
+    <t>Replacement and Installation of Generator Base Plate Adjusting Screw</t>
+  </si>
+  <si>
     <t>Replacement and Spare of Damaged Mechanical Seal</t>
   </si>
   <si>
     <t>Replacement and Spare of Worn-out Injector Nozzles</t>
   </si>
   <si>
+    <t>Replacement Bolts for Jacket Water Return Line</t>
+  </si>
+  <si>
+    <t>Replacement for Busted Battery Charger Fuse</t>
+  </si>
+  <si>
+    <t>Replacement for Damage Tool</t>
+  </si>
+  <si>
+    <t>Replacement in DG1 &amp; DG2 Governor Raise &amp; Lower Function</t>
+  </si>
+  <si>
+    <t>Replacement in Right Bank Bellow and Transition Piece</t>
+  </si>
+  <si>
     <t>Replacement Materials for Riser Pipes and Consumables for Cleaning of Pump</t>
   </si>
   <si>
+    <t>Replacement of Air Cooler Left &amp; Right Bank</t>
+  </si>
+  <si>
     <t>Replacement of Air Cooler O-Ring</t>
   </si>
   <si>
+    <t>Replacement of Battery Charger</t>
+  </si>
+  <si>
     <t>Replacement of Bearing for Spare Turning Gear Motor.</t>
   </si>
   <si>
+    <t>Replacement of Breaker from 3-Phase to Single Phase</t>
+  </si>
+  <si>
     <t>Replacement of Busted Light Bulbs</t>
   </si>
   <si>
+    <t>Replacement of Cable in 750KVA Station Transformer Feeder</t>
+  </si>
+  <si>
     <t>Replacement of Cooler Plate and Gasket for Lube Oil Cooler</t>
   </si>
   <si>
+    <t>Replacement of Corroded Bolts</t>
+  </si>
+  <si>
     <t>Replacement of Damage EPC41 Controller Card End Use</t>
   </si>
   <si>
@@ -886,18 +1246,45 @@
     <t>Replacement of damaged HDMI cable located at Bago Conference Room</t>
   </si>
   <si>
+    <t>Replacement of Defective Gauges in Fuel Module</t>
+  </si>
+  <si>
+    <t>Replacement of Defective Pressure Gauges in Fuel and Control Air System</t>
+  </si>
+  <si>
+    <t>Replacement of Defective/Malfunction Air Starting Solenoid Valve</t>
+  </si>
+  <si>
     <t>Replacement of Hydraulic Tensioning Jack Damaged Parts and Additional Hose</t>
   </si>
   <si>
+    <t>Replacement of Lube Oil Pump Bearing</t>
+  </si>
+  <si>
+    <t>Replacement of Non-Functional Pressure Gauges</t>
+  </si>
+  <si>
     <t>Replacement of Seals for Spare Jacket Water Pump</t>
   </si>
   <si>
     <t>Replacement of Worn-Out (Old) Injector Pop Tester</t>
   </si>
   <si>
+    <t>Replacement of Worn-Out Hand Tap</t>
+  </si>
+  <si>
     <t>Replacement on MGC3 Panel Main Breaker</t>
   </si>
   <si>
+    <t>Replacement Part &amp; Consumables For Battery Banks</t>
+  </si>
+  <si>
+    <t>Replacement Parts For Soft Water Pump</t>
+  </si>
+  <si>
+    <t>Replacement Shutdown Solenoid Valve for Engine Driven Fire Pump</t>
+  </si>
+  <si>
     <t>Reprogramming</t>
   </si>
   <si>
@@ -907,9 +1294,18 @@
     <t>Rethreading of Spare Main Lube Oil Pump</t>
   </si>
   <si>
+    <t>Retrofitting of 40kW Lube Oil Circulating Immersion Type Electric Heater</t>
+  </si>
+  <si>
     <t>Rewinding</t>
   </si>
   <si>
+    <t>Rewinding of Overhead Crane Hoist Motor Stator</t>
+  </si>
+  <si>
+    <t>Rewinding of Stator Hoist Motor</t>
+  </si>
+  <si>
     <t>Roof Replacement @ Auxiliary</t>
   </si>
   <si>
@@ -928,6 +1324,9 @@
     <t>Safety Gate Lock</t>
   </si>
   <si>
+    <t>Scrap Recovery</t>
+  </si>
+  <si>
     <t>Secondary Fire Exit</t>
   </si>
   <si>
@@ -943,28 +1342,40 @@
     <t>Servicing Generator</t>
   </si>
   <si>
+    <t>Servicing of Fuel Injectors</t>
+  </si>
+  <si>
     <t>Servicing of Lube Oil Purifiers and Replacement of Bolts</t>
   </si>
   <si>
     <t>Servicing of Primary &amp; Secondary Filters &amp; Reconditioning of Fuel Injector</t>
   </si>
   <si>
+    <t>Servicing of Spare Lube Oil Cooler Plates</t>
+  </si>
+  <si>
     <t>Servicing, Reconditioning and Automation of One (1) Unit Westfalia Lube Oil Purfier</t>
   </si>
   <si>
     <t>Sludge Tank Recovery, Common.</t>
   </si>
   <si>
+    <t>Socket Replacement at Sump Lighting</t>
+  </si>
+  <si>
     <t>Sounding Activities</t>
   </si>
   <si>
     <t>Source Air &amp; Ambient Air Monitoring as Per DENR Requirements / Compliance</t>
   </si>
   <si>
+    <t>Spare</t>
+  </si>
+  <si>
     <t>Spare Air Cooler</t>
   </si>
   <si>
-    <t>Spare Anti Condensate heater for DG1, DG 2 and DG 3 Generator Winding</t>
+    <t>Spare Anti Condensate Heater for Generator Winding</t>
   </si>
   <si>
     <t>Spare Fuel Injector</t>
@@ -973,9 +1384,21 @@
     <t>Spare Ideal Generator</t>
   </si>
   <si>
+    <t>Spare Part For Control Air Compressor</t>
+  </si>
+  <si>
+    <t>Spare Parts for LO Seperator</t>
+  </si>
+  <si>
+    <t>Spare Stator Cable</t>
+  </si>
+  <si>
     <t>Spare Stator Rewinding Enclosure</t>
   </si>
   <si>
+    <t>Special Tool For Deep Well Pipe Installation</t>
+  </si>
+  <si>
     <t>Special Tool, Pielstick</t>
   </si>
   <si>
@@ -988,12 +1411,18 @@
     <t>Station Service No. 2</t>
   </si>
   <si>
+    <t>Stator Terminal Lead Connection</t>
+  </si>
+  <si>
     <t>Steel Pole for Microwave Antenna</t>
   </si>
   <si>
     <t>Storage Area Enclosure</t>
   </si>
   <si>
+    <t>Substation Perimeter Lighting Re-Wiring</t>
+  </si>
+  <si>
     <t>Suction of Header Line</t>
   </si>
   <si>
@@ -1021,18 +1450,36 @@
     <t>Termination of Current Inputs</t>
   </si>
   <si>
+    <t>Testing &amp; Commissioning of Engine-Driven Fire Pump</t>
+  </si>
+  <si>
     <t>Testing Equipment</t>
   </si>
   <si>
+    <t>Testing of SEPAM Relay Current Transformer</t>
+  </si>
+  <si>
+    <t>Testing Solenoid Valve</t>
+  </si>
+  <si>
     <t>Testing/Sampling</t>
   </si>
   <si>
     <t>Threading of Lifting Tool</t>
   </si>
   <si>
+    <t>Time Synchronization During Dispatch</t>
+  </si>
+  <si>
+    <t>To Prevent Spreading of Viruses and Bacteria in the Workplace</t>
+  </si>
+  <si>
     <t>Tool For Engine Leak Down Test</t>
   </si>
   <si>
+    <t>Tools &amp; Consumables for Engine Alignment &amp; Grouting</t>
+  </si>
+  <si>
     <t>Tools Requirement for Repair at Air Duct.</t>
   </si>
   <si>
@@ -1042,6 +1489,9 @@
     <t>Training on Oil Spill Contingency Planning</t>
   </si>
   <si>
+    <t>Transfer and Modification</t>
+  </si>
+  <si>
     <t>Transferring of Panel</t>
   </si>
   <si>
@@ -1085,6 +1535,9 @@
   </si>
   <si>
     <t>Waste Heat Recovery Boilers Removal</t>
+  </si>
+  <si>
+    <t>Water System For Canteen &amp; Ladies Dorm</t>
   </si>
   <si>
     <t>Water Treatment</t>
@@ -1476,10 +1929,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B511"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B360" sqref="B360"/>
+      <selection activeCell="B511" sqref="B511"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3466,7 +3919,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -3474,7 +3927,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3482,7 +3935,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3490,7 +3943,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3498,7 +3951,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -3506,7 +3959,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -3514,7 +3967,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -3522,7 +3975,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -3530,7 +3983,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -3538,7 +3991,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -3546,7 +3999,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -3554,7 +4007,7 @@
         <v>257</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -3562,7 +4015,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -3570,7 +4023,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -3578,7 +4031,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -3586,7 +4039,7 @@
         <v>261</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -3594,7 +4047,7 @@
         <v>262</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -3602,7 +4055,7 @@
         <v>263</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -3610,7 +4063,7 @@
         <v>264</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -3618,7 +4071,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -3626,7 +4079,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -3634,7 +4087,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -3642,7 +4095,7 @@
         <v>268</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -3650,7 +4103,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -3658,7 +4111,7 @@
         <v>270</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -3666,7 +4119,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -3674,7 +4127,7 @@
         <v>272</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -3682,7 +4135,7 @@
         <v>273</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -3690,7 +4143,7 @@
         <v>274</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -3698,7 +4151,7 @@
         <v>275</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -3706,7 +4159,7 @@
         <v>276</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -3714,7 +4167,7 @@
         <v>277</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -3722,7 +4175,7 @@
         <v>278</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -3730,7 +4183,7 @@
         <v>279</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -3738,7 +4191,7 @@
         <v>280</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -3746,7 +4199,7 @@
         <v>281</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -3754,7 +4207,7 @@
         <v>282</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -3762,7 +4215,7 @@
         <v>283</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -3770,7 +4223,7 @@
         <v>284</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -3778,7 +4231,7 @@
         <v>285</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -3786,7 +4239,7 @@
         <v>286</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -3794,7 +4247,7 @@
         <v>287</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -3802,7 +4255,7 @@
         <v>288</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -3810,7 +4263,7 @@
         <v>289</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -3818,7 +4271,7 @@
         <v>290</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -3826,7 +4279,7 @@
         <v>291</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -3834,7 +4287,7 @@
         <v>292</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -3842,7 +4295,7 @@
         <v>293</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -3850,7 +4303,7 @@
         <v>294</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -3858,7 +4311,7 @@
         <v>295</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -3866,7 +4319,7 @@
         <v>296</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -3874,7 +4327,7 @@
         <v>297</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -3882,7 +4335,7 @@
         <v>298</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -3890,7 +4343,7 @@
         <v>299</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -3898,7 +4351,7 @@
         <v>300</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -3906,7 +4359,7 @@
         <v>301</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -3914,7 +4367,7 @@
         <v>302</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -3922,7 +4375,7 @@
         <v>303</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -3930,7 +4383,7 @@
         <v>304</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -3938,7 +4391,7 @@
         <v>305</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -3946,7 +4399,7 @@
         <v>306</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -3954,7 +4407,7 @@
         <v>307</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -3962,7 +4415,7 @@
         <v>308</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -3970,7 +4423,7 @@
         <v>309</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -3978,7 +4431,7 @@
         <v>310</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -3986,7 +4439,7 @@
         <v>311</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -3994,7 +4447,7 @@
         <v>312</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -4002,7 +4455,7 @@
         <v>313</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -4010,7 +4463,7 @@
         <v>314</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -4018,7 +4471,7 @@
         <v>315</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -4026,7 +4479,7 @@
         <v>316</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -4034,7 +4487,7 @@
         <v>317</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -4042,7 +4495,7 @@
         <v>318</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -4050,7 +4503,7 @@
         <v>319</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -4058,7 +4511,7 @@
         <v>320</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -4066,7 +4519,7 @@
         <v>321</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -4074,7 +4527,7 @@
         <v>322</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -4082,7 +4535,7 @@
         <v>323</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -4090,7 +4543,7 @@
         <v>324</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -4098,7 +4551,7 @@
         <v>325</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -4106,7 +4559,7 @@
         <v>326</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -4114,7 +4567,7 @@
         <v>327</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -4122,7 +4575,7 @@
         <v>328</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -4130,7 +4583,7 @@
         <v>329</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -4138,7 +4591,7 @@
         <v>330</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -4146,7 +4599,7 @@
         <v>331</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -4154,7 +4607,7 @@
         <v>332</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -4162,7 +4615,7 @@
         <v>333</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -4170,7 +4623,7 @@
         <v>334</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -4178,7 +4631,7 @@
         <v>335</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -4186,7 +4639,7 @@
         <v>336</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -4194,7 +4647,7 @@
         <v>337</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -4202,7 +4655,7 @@
         <v>338</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -4210,7 +4663,7 @@
         <v>339</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -4218,7 +4671,7 @@
         <v>340</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -4226,7 +4679,7 @@
         <v>341</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -4234,7 +4687,7 @@
         <v>342</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -4242,7 +4695,7 @@
         <v>343</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -4250,7 +4703,7 @@
         <v>344</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -4258,7 +4711,7 @@
         <v>345</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -4266,7 +4719,7 @@
         <v>346</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -4274,7 +4727,7 @@
         <v>347</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -4282,7 +4735,7 @@
         <v>348</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -4290,7 +4743,7 @@
         <v>349</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -4298,7 +4751,7 @@
         <v>350</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -4306,7 +4759,7 @@
         <v>351</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -4314,7 +4767,7 @@
         <v>352</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -4322,7 +4775,7 @@
         <v>353</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -4330,7 +4783,7 @@
         <v>354</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -4338,7 +4791,7 @@
         <v>355</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -4346,7 +4799,7 @@
         <v>356</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -4354,7 +4807,7 @@
         <v>357</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -4362,7 +4815,1215 @@
         <v>358</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
+      <c r="A361" s="5">
+        <v>359</v>
+      </c>
+      <c r="B361" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
+      <c r="A362" s="5">
+        <v>360</v>
+      </c>
+      <c r="B362" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
+      <c r="A363" s="5">
+        <v>361</v>
+      </c>
+      <c r="B363" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="A364" s="5">
+        <v>362</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
+      <c r="A365" s="5">
+        <v>363</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
+      <c r="A366" s="5">
+        <v>364</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
+      <c r="A367" s="5">
+        <v>365</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
+      <c r="A368" s="5">
+        <v>366</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
+      <c r="A369" s="5">
+        <v>367</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
+      <c r="A370" s="5">
+        <v>368</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
+      <c r="A371" s="5">
+        <v>369</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
+      <c r="A372" s="5">
+        <v>370</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
+      <c r="A373" s="5">
+        <v>371</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
+      <c r="A374" s="5">
+        <v>372</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
+      <c r="A375" s="5">
+        <v>373</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
+      <c r="A376" s="5">
+        <v>374</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
+      <c r="A377" s="5">
+        <v>375</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
+      <c r="A378" s="5">
+        <v>376</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="A379" s="5">
+        <v>377</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
+      <c r="A380" s="5">
+        <v>378</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
+      <c r="A381" s="5">
+        <v>379</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
+      <c r="A382" s="5">
+        <v>380</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
+      <c r="A383" s="5">
+        <v>381</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
+      <c r="A384" s="5">
+        <v>382</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
+      <c r="A385" s="5">
+        <v>383</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
+      <c r="A386" s="5">
+        <v>384</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
+      <c r="A387" s="5">
+        <v>385</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
+      <c r="A388" s="5">
+        <v>386</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
+      <c r="A389" s="5">
+        <v>387</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
+      <c r="A390" s="5">
+        <v>388</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
+      <c r="A391" s="5">
+        <v>389</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
+      <c r="A392" s="5">
+        <v>390</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
+      <c r="A393" s="5">
+        <v>391</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="A394" s="5">
+        <v>392</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
+      <c r="A395" s="5">
+        <v>393</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
+      <c r="A396" s="5">
+        <v>394</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
+      <c r="A397" s="5">
+        <v>395</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
+      <c r="A398" s="5">
+        <v>396</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2">
+      <c r="A399" s="5">
+        <v>397</v>
+      </c>
+      <c r="B399" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
+      <c r="A400" s="5">
+        <v>398</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
+      <c r="A401" s="5">
+        <v>399</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
+      <c r="A402" s="5">
+        <v>400</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
+      <c r="A403" s="5">
+        <v>401</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
+      <c r="A404" s="5">
+        <v>402</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
+      <c r="A405" s="5">
+        <v>403</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
+      <c r="A406" s="5">
+        <v>404</v>
+      </c>
+      <c r="B406" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
+      <c r="A407" s="5">
+        <v>405</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
+      <c r="A408" s="5">
+        <v>406</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="A409" s="5">
+        <v>407</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
+      <c r="A410" s="5">
+        <v>408</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
+      <c r="A411" s="5">
+        <v>409</v>
+      </c>
+      <c r="B411" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
+      <c r="A412" s="5">
+        <v>410</v>
+      </c>
+      <c r="B412" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
+      <c r="A413" s="5">
+        <v>411</v>
+      </c>
+      <c r="B413" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
+      <c r="A414" s="5">
+        <v>412</v>
+      </c>
+      <c r="B414" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
+      <c r="A415" s="5">
+        <v>413</v>
+      </c>
+      <c r="B415" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
+      <c r="A416" s="5">
+        <v>414</v>
+      </c>
+      <c r="B416" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
+      <c r="A417" s="5">
+        <v>415</v>
+      </c>
+      <c r="B417" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
+      <c r="A418" s="5">
+        <v>416</v>
+      </c>
+      <c r="B418" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2">
+      <c r="A419" s="5">
+        <v>417</v>
+      </c>
+      <c r="B419" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
+      <c r="A420" s="5">
+        <v>418</v>
+      </c>
+      <c r="B420" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
+      <c r="A421" s="5">
+        <v>419</v>
+      </c>
+      <c r="B421" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
+      <c r="A422" s="5">
+        <v>420</v>
+      </c>
+      <c r="B422" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
+      <c r="A423" s="5">
+        <v>421</v>
+      </c>
+      <c r="B423" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="A424" s="5">
+        <v>422</v>
+      </c>
+      <c r="B424" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
+      <c r="A425" s="5">
+        <v>423</v>
+      </c>
+      <c r="B425" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2">
+      <c r="A426" s="5">
+        <v>424</v>
+      </c>
+      <c r="B426" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
+      <c r="A427" s="5">
+        <v>425</v>
+      </c>
+      <c r="B427" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
+      <c r="A428" s="5">
+        <v>426</v>
+      </c>
+      <c r="B428" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2">
+      <c r="A429" s="5">
+        <v>427</v>
+      </c>
+      <c r="B429" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2">
+      <c r="A430" s="5">
+        <v>428</v>
+      </c>
+      <c r="B430" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2">
+      <c r="A431" s="5">
+        <v>429</v>
+      </c>
+      <c r="B431" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2">
+      <c r="A432" s="5">
+        <v>430</v>
+      </c>
+      <c r="B432" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2">
+      <c r="A433" s="5">
+        <v>431</v>
+      </c>
+      <c r="B433" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2">
+      <c r="A434" s="5">
+        <v>432</v>
+      </c>
+      <c r="B434" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2">
+      <c r="A435" s="5">
+        <v>433</v>
+      </c>
+      <c r="B435" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
+      <c r="A436" s="5">
+        <v>434</v>
+      </c>
+      <c r="B436" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
+      <c r="A437" s="5">
+        <v>435</v>
+      </c>
+      <c r="B437" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
+      <c r="A438" s="5">
+        <v>436</v>
+      </c>
+      <c r="B438" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="A439" s="5">
+        <v>437</v>
+      </c>
+      <c r="B439" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
+      <c r="A440" s="5">
+        <v>438</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
+      <c r="A441" s="5">
+        <v>439</v>
+      </c>
+      <c r="B441" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2">
+      <c r="A442" s="5">
+        <v>440</v>
+      </c>
+      <c r="B442" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" s="5">
+        <v>441</v>
+      </c>
+      <c r="B443" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
+      <c r="A444" s="5">
+        <v>442</v>
+      </c>
+      <c r="B444" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
+      <c r="A445" s="5">
+        <v>443</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" s="5">
+        <v>444</v>
+      </c>
+      <c r="B446" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
+      <c r="A447" s="5">
+        <v>445</v>
+      </c>
+      <c r="B447" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
+      <c r="A448" s="5">
+        <v>446</v>
+      </c>
+      <c r="B448" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
+      <c r="A449" s="5">
+        <v>447</v>
+      </c>
+      <c r="B449" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
+      <c r="A450" s="5">
+        <v>448</v>
+      </c>
+      <c r="B450" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2">
+      <c r="A451" s="5">
+        <v>449</v>
+      </c>
+      <c r="B451" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
+      <c r="A452" s="5">
+        <v>450</v>
+      </c>
+      <c r="B452" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
+      <c r="A453" s="5">
+        <v>451</v>
+      </c>
+      <c r="B453" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="A454" s="5">
+        <v>452</v>
+      </c>
+      <c r="B454" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
+      <c r="A455" s="5">
+        <v>453</v>
+      </c>
+      <c r="B455" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
+      <c r="A456" s="5">
+        <v>454</v>
+      </c>
+      <c r="B456" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
+      <c r="A457" s="5">
+        <v>455</v>
+      </c>
+      <c r="B457" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2">
+      <c r="A458" s="5">
+        <v>456</v>
+      </c>
+      <c r="B458" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
+      <c r="A459" s="5">
+        <v>457</v>
+      </c>
+      <c r="B459" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
+      <c r="A460" s="5">
+        <v>458</v>
+      </c>
+      <c r="B460" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
+      <c r="A461" s="5">
+        <v>459</v>
+      </c>
+      <c r="B461" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
+      <c r="A462" s="5">
+        <v>460</v>
+      </c>
+      <c r="B462" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
+      <c r="A463" s="5">
+        <v>461</v>
+      </c>
+      <c r="B463" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2">
+      <c r="A464" s="5">
+        <v>462</v>
+      </c>
+      <c r="B464" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
+      <c r="A465" s="5">
+        <v>463</v>
+      </c>
+      <c r="B465" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2">
+      <c r="A466" s="5">
+        <v>464</v>
+      </c>
+      <c r="B466" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
+      <c r="A467" s="5">
+        <v>465</v>
+      </c>
+      <c r="B467" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
+      <c r="A468" s="5">
+        <v>466</v>
+      </c>
+      <c r="B468" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="A469" s="5">
+        <v>467</v>
+      </c>
+      <c r="B469" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
+      <c r="A470" s="5">
+        <v>468</v>
+      </c>
+      <c r="B470" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
+      <c r="A471" s="5">
+        <v>469</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
+      <c r="A472" s="5">
+        <v>470</v>
+      </c>
+      <c r="B472" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" s="5">
+        <v>471</v>
+      </c>
+      <c r="B473" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
+      <c r="A474" s="5">
+        <v>472</v>
+      </c>
+      <c r="B474" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2">
+      <c r="A475" s="5">
+        <v>473</v>
+      </c>
+      <c r="B475" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2">
+      <c r="A476" s="5">
+        <v>474</v>
+      </c>
+      <c r="B476" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2">
+      <c r="A477" s="5">
+        <v>475</v>
+      </c>
+      <c r="B477" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2">
+      <c r="A478" s="5">
+        <v>476</v>
+      </c>
+      <c r="B478" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2">
+      <c r="A479" s="5">
+        <v>477</v>
+      </c>
+      <c r="B479" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2">
+      <c r="A480" s="5">
+        <v>478</v>
+      </c>
+      <c r="B480" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2">
+      <c r="A481" s="5">
+        <v>479</v>
+      </c>
+      <c r="B481" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2">
+      <c r="A482" s="5">
+        <v>480</v>
+      </c>
+      <c r="B482" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2">
+      <c r="A483" s="5">
+        <v>481</v>
+      </c>
+      <c r="B483" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="A484" s="5">
+        <v>482</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2">
+      <c r="A485" s="5">
+        <v>483</v>
+      </c>
+      <c r="B485" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2">
+      <c r="A486" s="5">
+        <v>484</v>
+      </c>
+      <c r="B486" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2">
+      <c r="A487" s="5">
+        <v>485</v>
+      </c>
+      <c r="B487" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2">
+      <c r="A488" s="5">
+        <v>486</v>
+      </c>
+      <c r="B488" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2">
+      <c r="A489" s="5">
+        <v>487</v>
+      </c>
+      <c r="B489" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2">
+      <c r="A490" s="5">
+        <v>488</v>
+      </c>
+      <c r="B490" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2">
+      <c r="A491" s="5">
+        <v>489</v>
+      </c>
+      <c r="B491" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2">
+      <c r="A492" s="5">
+        <v>490</v>
+      </c>
+      <c r="B492" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2">
+      <c r="A493" s="5">
+        <v>491</v>
+      </c>
+      <c r="B493" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2">
+      <c r="A494" s="5">
+        <v>492</v>
+      </c>
+      <c r="B494" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2">
+      <c r="A495" s="5">
+        <v>493</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2">
+      <c r="A496" s="5">
+        <v>494</v>
+      </c>
+      <c r="B496" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2">
+      <c r="A497" s="5">
+        <v>495</v>
+      </c>
+      <c r="B497" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2">
+      <c r="A498" s="5">
+        <v>496</v>
+      </c>
+      <c r="B498" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2">
+      <c r="A499" s="5">
+        <v>497</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2">
+      <c r="A500" s="5">
+        <v>498</v>
+      </c>
+      <c r="B500" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2">
+      <c r="A501" s="5">
+        <v>499</v>
+      </c>
+      <c r="B501" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2">
+      <c r="A502" s="5">
+        <v>500</v>
+      </c>
+      <c r="B502" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2">
+      <c r="A503" s="5">
+        <v>501</v>
+      </c>
+      <c r="B503" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2">
+      <c r="A504" s="5">
+        <v>502</v>
+      </c>
+      <c r="B504" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2">
+      <c r="A505" s="5">
+        <v>503</v>
+      </c>
+      <c r="B505" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2">
+      <c r="A506" s="5">
+        <v>504</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2">
+      <c r="A507" s="5">
+        <v>505</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2">
+      <c r="A508" s="5">
+        <v>506</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2">
+      <c r="A509" s="5">
+        <v>507</v>
+      </c>
+      <c r="B509" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2">
+      <c r="A510" s="5">
+        <v>508</v>
+      </c>
+      <c r="B510" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2">
+      <c r="A511" s="5">
+        <v>509</v>
+      </c>
+      <c r="B511" s="2" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>